<commit_message>
added classes and properties for v1.1.0
</commit_message>
<xml_diff>
--- a/requirements/requirements.xlsx
+++ b/requirements/requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="226">
   <si>
     <t>CQ ID</t>
   </si>
@@ -225,12 +225,6 @@
     <t>sd:SoftwareConfiguration, sd:hasSampleExecution, sd:SampleExecution(prov:Activity)</t>
   </si>
   <si>
-    <t>prov:Activity, prov:used, sd:SampleInput(prov:Entity), opmw:correspondsToTemplateArtifact</t>
-  </si>
-  <si>
-    <t>sd:SoftwareConfiguration, sd:hasSampleResult, sd:sampleResult (prov:Entity)</t>
-  </si>
-  <si>
     <t>sd:SoftwareConfiguration, sd:hasOutput, sd:DatasetSpecification</t>
   </si>
   <si>
@@ -354,9 +348,6 @@
     <t>sd:Software;sd:shortDescription (extension of schema:description);xsd:string</t>
   </si>
   <si>
-    <t>sd:SoftwareConfiguration, opmw:WorkflowExecutionProcess, sd:Container sd:hasInvocationCommand, xsd:string</t>
-  </si>
-  <si>
     <t>sd:Software,schema:description,xsd:string</t>
   </si>
   <si>
@@ -426,9 +417,6 @@
     <t>Trust on who published the software</t>
   </si>
   <si>
-    <t>sd:Software, sd:contactDetails, xsd:string</t>
-  </si>
-  <si>
     <t>Could include a contact person or just details, mailing lists, etc. This field is included in case a person is not provided</t>
   </si>
   <si>
@@ -612,9 +600,6 @@
     <t>sd:SoftwareConfiguration, sd:hasQualifiedInput, sd:hasQualifiedOutput, sd:QualifiedInput, sd:QualifiedOutput</t>
   </si>
   <si>
-    <t>sd:SoftwareConfiguration, sd:hasAssumptions, sxsd:tring</t>
-  </si>
-  <si>
     <t>sd:DatasetSpecification, sd:hasPresentation,  sd:VariablePresentation</t>
   </si>
   <si>
@@ -646,13 +631,79 @@
   </si>
   <si>
     <t>sd:Container, schema:name, xsd:string</t>
+  </si>
+  <si>
+    <t>Needed to address common questions about the software</t>
+  </si>
+  <si>
+    <t>sd:Software, hasFAQ, xsd:anyURI</t>
+  </si>
+  <si>
+    <t>Is there an FAQ guide to troubleshoot common errors?</t>
+  </si>
+  <si>
+    <t>Sometimes you may have several scripts to wrap a component: e.g., a main script that invokes a software</t>
+  </si>
+  <si>
+    <t>Is an input/output to this software an image?</t>
+  </si>
+  <si>
+    <t>What is this software useful for?</t>
+  </si>
+  <si>
+    <t>What are typical data sources for this software?</t>
+  </si>
+  <si>
+    <t>sd:hasTypicalDataSources</t>
+  </si>
+  <si>
+    <t>Used to guide users towards the right data sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd:SoftwareConfiguration, sd:hasInput,sd:Image </t>
+  </si>
+  <si>
+    <t>It is useful to identify image files that can be visualized</t>
+  </si>
+  <si>
+    <t>sd:Software, sd:hasPurpose, xsd:string</t>
+  </si>
+  <si>
+    <t>Used to define the main purpose of the model. Note that the purpose is not a description</t>
+  </si>
+  <si>
+    <t>sd:Software, sd:supportDetails, xsd:string</t>
+  </si>
+  <si>
+    <t>How long is this software supposed to take?</t>
+  </si>
+  <si>
+    <t>An estimation on how long the software takes to run</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>prov:Activity, prov:used, sd:SampleResource(prov:Entity), opmw:correspondsToTemplateArtifact</t>
+  </si>
+  <si>
+    <t>sd:SoftwareConfiguration, sd:hasSampleResource, sd:sampleResult (prov:Entity)</t>
+  </si>
+  <si>
+    <t>sd:SoftwareConfiguration, sd:hasAssumption, sxsd:tring</t>
+  </si>
+  <si>
+    <t>Needed to know precisely how the software has been invoked in the sample execution</t>
+  </si>
+  <si>
+    <t>sd:SoftwareConfiguration, opmw:WorkflowExecutionProcess, sd:hasInvocationCommand, xsd:string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,8 +720,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -689,8 +754,18 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -764,6 +839,21 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,11 +935,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -887,9 +1025,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -898,48 +1033,80 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1218,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S204"/>
+  <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1247,7 +1414,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1262,10 +1429,10 @@
       <c r="C2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="13"/>
@@ -1282,7 +1449,7 @@
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ2</v>
@@ -1293,10 +1460,10 @@
       <c r="C3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="13"/>
@@ -1324,11 +1491,11 @@
       <c r="C4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>116</v>
+      <c r="D4" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>113</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -1353,13 +1520,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>117</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -1384,13 +1551,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>117</v>
+        <v>124</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -1415,13 +1582,13 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>117</v>
+        <v>121</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -1446,13 +1613,13 @@
         <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>117</v>
+        <v>122</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1468,21 +1635,21 @@
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
     </row>
-    <row r="9" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="25"/>
+        <v>123</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="23"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -1503,15 +1670,15 @@
         <v>CQ9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="25"/>
+        <v>126</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="23"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -1532,15 +1699,15 @@
         <v>CQ10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="25"/>
+        <v>128</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="23"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -1561,16 +1728,16 @@
         <v>CQ11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>117</v>
+        <v>129</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -1586,7 +1753,7 @@
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
     </row>
-    <row r="13" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ12</v>
@@ -1595,13 +1762,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>117</v>
+        <v>131</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1626,12 +1793,12 @@
         <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="13"/>
@@ -1648,7 +1815,7 @@
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
     </row>
-    <row r="15" spans="1:18" s="7" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ14</v>
@@ -1657,13 +1824,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>134</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -1679,7 +1846,7 @@
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
     </row>
-    <row r="16" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ15</v>
@@ -1688,12 +1855,12 @@
         <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="13"/>
@@ -1719,12 +1886,12 @@
         <v>32</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="13"/>
@@ -1750,13 +1917,13 @@
         <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>144</v>
+        <v>139</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -1772,7 +1939,7 @@
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
     </row>
-    <row r="19" spans="1:18" s="7" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ18</v>
@@ -1781,12 +1948,12 @@
         <v>34</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="13"/>
@@ -1809,15 +1976,15 @@
         <v>CQ19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="23" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="13"/>
@@ -1834,7 +2001,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
     </row>
-    <row r="21" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ20</v>
@@ -1843,12 +2010,12 @@
         <v>35</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>65</v>
       </c>
       <c r="F21" s="13"/>
@@ -1865,7 +2032,7 @@
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
     </row>
-    <row r="22" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ21</v>
@@ -1874,13 +2041,13 @@
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>155</v>
+        <v>149</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>151</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
@@ -1905,12 +2072,12 @@
         <v>37</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="13"/>
@@ -1927,7 +2094,7 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
     </row>
-    <row r="24" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ23</v>
@@ -1936,12 +2103,12 @@
         <v>38</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>49</v>
       </c>
       <c r="F24" s="13"/>
@@ -1958,7 +2125,7 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
     </row>
-    <row r="25" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ24</v>
@@ -1967,13 +2134,13 @@
         <v>39</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>161</v>
+        <v>156</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -1989,7 +2156,7 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
     </row>
-    <row r="26" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ25</v>
@@ -1998,13 +2165,13 @@
         <v>40</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -2020,22 +2187,22 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
     </row>
-    <row r="27" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E27" s="25" t="s">
         <v>161</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -2057,15 +2224,15 @@
         <v>CQ27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="E28" s="18"/>
+        <v>164</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="17"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
@@ -2086,15 +2253,15 @@
         <v>CQ28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="18"/>
+        <v>165</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="17"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
@@ -2115,15 +2282,15 @@
         <v>CQ29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="E30" s="18"/>
+        <v>166</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="17"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
@@ -2144,15 +2311,15 @@
         <v>CQ30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E31" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" s="31" t="s">
         <v>22</v>
       </c>
       <c r="F31" s="13"/>
@@ -2180,10 +2347,10 @@
       <c r="C32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="26" t="s">
+      <c r="D32" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="24" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2196,16 +2363,16 @@
         <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ33</v>
@@ -2214,12 +2381,12 @@
         <v>41</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="31" t="s">
         <v>44</v>
       </c>
       <c r="F34" s="13"/>
@@ -2236,7 +2403,7 @@
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
     </row>
-    <row r="35" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" s="7" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="str">
         <f t="shared" si="0"/>
         <v>CQ34</v>
@@ -2245,12 +2412,12 @@
         <v>57</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="25"/>
+        <v>221</v>
+      </c>
+      <c r="E35" s="23"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2265,21 +2432,21 @@
       <c r="Q35" s="13"/>
       <c r="R35" s="13"/>
     </row>
-    <row r="36" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="str">
-        <f t="shared" ref="A36:A64" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
+        <f t="shared" ref="A36:A69" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
         <v>CQ35</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" s="25"/>
+        <v>175</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" s="23"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
@@ -2303,12 +2470,12 @@
         <v>59</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="25"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
@@ -2323,7 +2490,7 @@
       <c r="Q37" s="13"/>
       <c r="R37" s="13"/>
     </row>
-    <row r="38" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ37</v>
@@ -2332,12 +2499,12 @@
         <v>42</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E38" s="25"/>
+        <v>178</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="E38" s="23"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
@@ -2361,12 +2528,12 @@
         <v>43</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E39" s="32"/>
+        <v>179</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="E39" s="30"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
@@ -2381,7 +2548,7 @@
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
     </row>
-    <row r="40" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ39</v>
@@ -2390,13 +2557,13 @@
         <v>48</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D40" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>185</v>
+      <c r="E40" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
@@ -2412,7 +2579,7 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
     </row>
-    <row r="41" spans="1:18" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ40</v>
@@ -2423,11 +2590,11 @@
       <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>187</v>
+      <c r="D41" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>183</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
@@ -2443,103 +2610,103 @@
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
     </row>
-    <row r="42" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="30" t="str">
+    <row r="42" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="28" t="str">
         <f t="shared" si="1"/>
         <v>CQ41</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>187</v>
+      <c r="D42" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="66" x14ac:dyDescent="0.3">
-      <c r="A43" s="30" t="str">
+      <c r="A43" s="28" t="str">
         <f t="shared" si="1"/>
         <v>CQ42</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>188</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="35"/>
+      <c r="B43" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="D43" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="str">
+      <c r="A44" s="28" t="str">
         <f t="shared" si="1"/>
         <v>CQ43</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="35"/>
+      <c r="B44" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="30" t="str">
+      <c r="A45" s="28" t="str">
         <f t="shared" si="1"/>
         <v>CQ44</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E45" s="35"/>
-    </row>
-    <row r="46" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="str">
+      <c r="B45" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" s="33"/>
+    </row>
+    <row r="46" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="28" t="str">
         <f t="shared" si="1"/>
         <v>CQ45</v>
       </c>
-      <c r="B46" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" s="35"/>
-    </row>
-    <row r="47" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B46" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E47" s="35"/>
+        <v>97</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D47" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="str">
@@ -2547,16 +2714,16 @@
         <v>CQ47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E48" s="34" t="s">
-        <v>195</v>
+      <c r="D48" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="E48" s="32" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:19" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2569,7 +2736,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>63</v>
@@ -2581,15 +2748,15 @@
         <v>CQ49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E50" s="27"/>
+        <v>71</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="str">
@@ -2597,15 +2764,15 @@
         <v>CQ50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E51" s="27" t="s">
+      <c r="D51" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="E51" s="25" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2621,10 +2788,10 @@
         <v>7</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>106</v>
+        <v>195</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:19" s="7" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2638,11 +2805,11 @@
       <c r="C53" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>201</v>
+      <c r="D53" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>196</v>
       </c>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
@@ -2669,10 +2836,10 @@
       <c r="C54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E54" s="25"/>
+      <c r="D54" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="E54" s="23"/>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
@@ -2687,22 +2854,22 @@
       <c r="Q54" s="13"/>
       <c r="R54" s="13"/>
     </row>
-    <row r="55" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="25" t="s">
         <v>77</v>
-      </c>
-      <c r="E55" s="27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
@@ -2711,16 +2878,16 @@
         <v>CQ55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E56" s="27" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="D56" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="52.8" x14ac:dyDescent="0.3">
@@ -2729,29 +2896,31 @@
         <v>CQ56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E57" s="25"/>
-    </row>
-    <row r="58" spans="1:19" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="E57" s="23"/>
+    </row>
+    <row r="58" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E58" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="E58" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2763,15 +2932,17 @@
       <c r="B59" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C59" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="str">
         <f t="shared" si="1"/>
         <v>CQ59</v>
@@ -2780,13 +2951,13 @@
         <v>16</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E60" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="D60" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
@@ -2798,12 +2969,12 @@
         <v>17</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="E61" s="25"/>
+        <v>199</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61" s="23"/>
     </row>
     <row r="62" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="str">
@@ -2814,12 +2985,12 @@
         <v>18</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E62" s="25"/>
+        <v>199</v>
+      </c>
+      <c r="D62" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E62" s="23"/>
     </row>
     <row r="63" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="str">
@@ -2830,28 +3001,28 @@
         <v>19</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="E63" s="25"/>
-    </row>
-    <row r="64" spans="1:19" s="19" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="21" t="str">
+        <v>199</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="E63" s="23"/>
+    </row>
+    <row r="64" spans="1:19" s="18" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="20" t="str">
         <f t="shared" si="1"/>
         <v>CQ63</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E64" s="18"/>
+      <c r="C64" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D64" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="E64" s="35"/>
       <c r="F64" s="16"/>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
@@ -2867,40 +3038,87 @@
       <c r="R64" s="16"/>
       <c r="S64" s="16"/>
     </row>
-    <row r="65" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-    </row>
-    <row r="66" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="14"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="9"/>
-    </row>
-    <row r="67" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="9"/>
-    </row>
-    <row r="68" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
+    <row r="65" spans="1:5" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ64</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="1:5" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ65</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="1:5" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ66</v>
+      </c>
+      <c r="B67" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" s="11"/>
+    </row>
+    <row r="68" spans="1:5" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ67</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E68" s="37" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="69" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
+      <c r="A69" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ68</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="E69" s="17"/>
     </row>
     <row r="70" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="14"/>
@@ -2923,19 +3141,19 @@
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="14"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-    </row>
-    <row r="74" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+    </row>
+    <row r="74" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="14"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
     </row>
     <row r="75" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="14"/>
@@ -2974,113 +3192,113 @@
     </row>
     <row r="80" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="14"/>
-      <c r="B80" s="15"/>
+      <c r="B80" s="19"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15"/>
     </row>
     <row r="81" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="14"/>
-      <c r="B81" s="15"/>
+      <c r="B81" s="19"/>
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
     </row>
     <row r="82" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="14"/>
-      <c r="B82" s="20"/>
+      <c r="B82" s="19"/>
       <c r="C82" s="15"/>
       <c r="D82" s="15"/>
       <c r="E82" s="15"/>
     </row>
     <row r="83" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
-      <c r="B83" s="20"/>
+      <c r="B83" s="19"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
     </row>
     <row r="84" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="14"/>
-      <c r="B84" s="20"/>
+      <c r="B84" s="19"/>
       <c r="C84" s="15"/>
       <c r="D84" s="15"/>
       <c r="E84" s="15"/>
     </row>
     <row r="85" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="14"/>
-      <c r="B85" s="20"/>
+      <c r="B85" s="19"/>
       <c r="C85" s="15"/>
       <c r="D85" s="15"/>
       <c r="E85" s="15"/>
     </row>
     <row r="86" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="14"/>
-      <c r="B86" s="20"/>
+      <c r="B86" s="19"/>
       <c r="C86" s="15"/>
       <c r="D86" s="15"/>
       <c r="E86" s="15"/>
     </row>
     <row r="87" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="14"/>
-      <c r="B87" s="20"/>
+      <c r="B87" s="19"/>
       <c r="C87" s="15"/>
       <c r="D87" s="15"/>
       <c r="E87" s="15"/>
     </row>
     <row r="88" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="14"/>
-      <c r="B88" s="20"/>
+      <c r="B88" s="19"/>
       <c r="C88" s="15"/>
       <c r="D88" s="15"/>
       <c r="E88" s="15"/>
     </row>
     <row r="89" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="14"/>
-      <c r="B89" s="20"/>
+      <c r="B89" s="19"/>
       <c r="C89" s="15"/>
       <c r="D89" s="15"/>
       <c r="E89" s="15"/>
     </row>
     <row r="90" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="14"/>
-      <c r="B90" s="20"/>
+      <c r="B90" s="19"/>
       <c r="C90" s="15"/>
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
     </row>
     <row r="91" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="14"/>
-      <c r="B91" s="20"/>
+      <c r="B91" s="19"/>
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
     </row>
     <row r="92" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="14"/>
-      <c r="B92" s="20"/>
+      <c r="B92" s="19"/>
       <c r="C92" s="15"/>
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
     </row>
     <row r="93" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="14"/>
-      <c r="B93" s="20"/>
+      <c r="B93" s="15"/>
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
     </row>
     <row r="94" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="14"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="15"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
       <c r="D94" s="15"/>
       <c r="E94" s="15"/>
     </row>
     <row r="95" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="14"/>
-      <c r="B95" s="15"/>
-      <c r="C95" s="15"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
       <c r="D95" s="15"/>
       <c r="E95" s="15"/>
     </row>
@@ -3094,7 +3312,7 @@
     <row r="97" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="14"/>
       <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
+      <c r="C97" s="9"/>
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
     </row>
@@ -3108,7 +3326,7 @@
     <row r="99" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="14"/>
       <c r="B99" s="12"/>
-      <c r="C99" s="9"/>
+      <c r="C99" s="12"/>
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
     </row>
@@ -3135,15 +3353,15 @@
     </row>
     <row r="103" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="14"/>
-      <c r="B103" s="12"/>
-      <c r="C103" s="12"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="15"/>
       <c r="D103" s="15"/>
       <c r="E103" s="15"/>
     </row>
     <row r="104" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="14"/>
-      <c r="B104" s="12"/>
-      <c r="C104" s="12"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="15"/>
       <c r="D104" s="15"/>
       <c r="E104" s="15"/>
     </row>
@@ -3833,20 +4051,6 @@
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
     </row>
-    <row r="203" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="14"/>
-      <c r="B203" s="15"/>
-      <c r="C203" s="15"/>
-      <c r="D203" s="15"/>
-      <c r="E203" s="15"/>
-    </row>
-    <row r="204" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="14"/>
-      <c r="B204" s="15"/>
-      <c r="C204" s="15"/>
-      <c r="D204" s="15"/>
-      <c r="E204" s="15"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a classand updated requirements
</commit_message>
<xml_diff>
--- a/requirements/requirements.xlsx
+++ b/requirements/requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="239">
   <si>
     <t>CQ ID</t>
   </si>
@@ -210,9 +210,6 @@
     <t>prov:Activity, prov:wasGeneratedBy, prov:Entity, opmw:correspondsToTemplateArtifact</t>
   </si>
   <si>
-    <t>Not yet implemented, will be implemented and aligned to CWL in the next version</t>
-  </si>
-  <si>
     <t>Formats may be aligned to other ontologies, such as EDAM and Wikidata</t>
   </si>
   <si>
@@ -712,13 +709,40 @@
   </si>
   <si>
     <t>Which execution(s) were used to create a software visualization</t>
+  </si>
+  <si>
+    <t>What is the index of an input in a configuration?</t>
+  </si>
+  <si>
+    <t>What is the index of an output in a configuration?</t>
+  </si>
+  <si>
+    <t>Source: WINGS</t>
+  </si>
+  <si>
+    <t>What is the inex of a parameter in a configuration</t>
+  </si>
+  <si>
+    <t>When a configuration has several inputs of the same type, they could adopt different positions in the execution of a component. This property captures that relationship. The role is not enough because there could be two inputs with the same role.</t>
+  </si>
+  <si>
+    <t>Requirement not necessary as a DatasetSpecification already acts as a qualified relationship</t>
+  </si>
+  <si>
+    <t>Requirement not necessary s DatasetOutputsation already acts s t presentation relationship</t>
+  </si>
+  <si>
+    <t>Requirement not necessary s it DatasetAppearsation already acts s i short relationship</t>
+  </si>
+  <si>
+    <t>Requirement not necessary as script DatasetUsedation already acts as t invocation relationship</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +772,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1002,7 +1037,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1125,6 +1160,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1411,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1454,7 +1495,7 @@
         <v>54</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>22</v>
@@ -1485,7 +1526,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>22</v>
@@ -1516,10 +1557,10 @@
         <v>52</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -1544,13 +1585,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="E5" s="23" t="s">
         <v>116</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>117</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -1575,13 +1616,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -1606,13 +1647,13 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -1637,13 +1678,13 @@
         <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1665,13 +1706,13 @@
         <v>CQ8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="13"/>
@@ -1694,13 +1735,13 @@
         <v>CQ9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="13"/>
@@ -1723,13 +1764,13 @@
         <v>CQ10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="13"/>
@@ -1752,16 +1793,16 @@
         <v>CQ11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -1786,13 +1827,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1817,10 +1858,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>22</v>
@@ -1848,13 +1889,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="40" t="s">
         <v>133</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>134</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -1879,10 +1920,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>22</v>
@@ -1910,10 +1951,10 @@
         <v>32</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="39" t="s">
         <v>137</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>138</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>22</v>
@@ -1941,13 +1982,13 @@
         <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>139</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>140</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -1972,10 +2013,10 @@
         <v>34</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="39" t="s">
         <v>142</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>143</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>22</v>
@@ -2000,16 +2041,16 @@
         <v>CQ19</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>145</v>
-      </c>
       <c r="E20" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -2034,13 +2075,13 @@
         <v>35</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -2065,13 +2106,13 @@
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="E22" s="23" t="s">
         <v>150</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>151</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
@@ -2096,10 +2137,10 @@
         <v>37</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>22</v>
@@ -2127,10 +2168,10 @@
         <v>38</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>49</v>
@@ -2158,13 +2199,13 @@
         <v>39</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>156</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>157</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -2189,13 +2230,13 @@
         <v>40</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -2217,16 +2258,16 @@
         <v>CQ26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="39" t="s">
-        <v>162</v>
-      </c>
       <c r="E27" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -2248,13 +2289,13 @@
         <v>CQ27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="13"/>
@@ -2277,13 +2318,13 @@
         <v>CQ28</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="44" t="s">
         <v>105</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>106</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="13"/>
@@ -2306,13 +2347,13 @@
         <v>CQ29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="44" t="s">
         <v>166</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>167</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="13"/>
@@ -2335,13 +2376,13 @@
         <v>CQ30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E31" s="31" t="s">
         <v>22</v>
@@ -2372,7 +2413,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>46</v>
@@ -2387,13 +2428,13 @@
         <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>171</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2405,10 +2446,10 @@
         <v>41</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>44</v>
@@ -2436,10 +2477,10 @@
         <v>57</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="13"/>
@@ -2458,17 +2499,17 @@
     </row>
     <row r="36" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="str">
-        <f t="shared" ref="A36:A73" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
+        <f t="shared" ref="A36:A76" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
         <v>CQ35</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="13"/>
@@ -2494,7 +2535,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>62</v>
@@ -2523,10 +2564,10 @@
         <v>42</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E38" s="23"/>
       <c r="F38" s="13"/>
@@ -2552,10 +2593,10 @@
         <v>43</v>
       </c>
       <c r="C39" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" s="39" t="s">
         <v>179</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>180</v>
       </c>
       <c r="E39" s="30"/>
       <c r="F39" s="13"/>
@@ -2581,13 +2622,13 @@
         <v>48</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D40" s="44" t="s">
         <v>53</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
@@ -2615,10 +2656,10 @@
         <v>5</v>
       </c>
       <c r="D41" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
@@ -2646,10 +2687,10 @@
         <v>8</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="66" x14ac:dyDescent="0.3">
@@ -2658,13 +2699,13 @@
         <v>CQ42</v>
       </c>
       <c r="B43" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="44" t="s">
         <v>92</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="D43" s="44" t="s">
-        <v>93</v>
       </c>
       <c r="E43" s="33"/>
     </row>
@@ -2674,13 +2715,13 @@
         <v>CQ43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E44" s="33"/>
     </row>
@@ -2690,13 +2731,13 @@
         <v>CQ44</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="21" t="s">
         <v>189</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>190</v>
       </c>
       <c r="E45" s="33"/>
     </row>
@@ -2706,13 +2747,13 @@
         <v>CQ45</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D46" s="44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E46" s="33"/>
     </row>
@@ -2722,13 +2763,13 @@
         <v>CQ46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D47" s="44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E47" s="33"/>
     </row>
@@ -2738,16 +2779,16 @@
         <v>CQ47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:19" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2755,15 +2796,15 @@
         <f t="shared" si="1"/>
         <v>CQ48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>63</v>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" s="49" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="39.6" x14ac:dyDescent="0.3">
@@ -2772,13 +2813,13 @@
         <v>CQ49</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D50" s="39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E50" s="25"/>
     </row>
@@ -2788,16 +2829,16 @@
         <v>CQ50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="39.6" x14ac:dyDescent="0.3">
@@ -2806,16 +2847,16 @@
         <v>CQ51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:19" s="7" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2830,10 +2871,10 @@
         <v>10</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
@@ -2861,7 +2902,7 @@
         <v>12</v>
       </c>
       <c r="D54" s="39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E54" s="23"/>
       <c r="F54" s="13"/>
@@ -2884,16 +2925,16 @@
         <v>CQ54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
@@ -2902,16 +2943,16 @@
         <v>CQ55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="52.8" x14ac:dyDescent="0.3">
@@ -2920,13 +2961,13 @@
         <v>CQ56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="39" t="s">
         <v>82</v>
-      </c>
-      <c r="D57" s="39" t="s">
-        <v>83</v>
       </c>
       <c r="E57" s="23"/>
     </row>
@@ -2936,13 +2977,13 @@
         <v>CQ57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" s="39" t="s">
         <v>224</v>
-      </c>
-      <c r="D58" s="39" t="s">
-        <v>225</v>
       </c>
       <c r="E58" s="23" t="s">
         <v>22</v>
@@ -2957,13 +2998,13 @@
         <v>15</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D59" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -2975,13 +3016,13 @@
         <v>16</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D60" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
@@ -2993,10 +3034,10 @@
         <v>17</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D61" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E61" s="23"/>
     </row>
@@ -3009,10 +3050,10 @@
         <v>18</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D62" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E62" s="23"/>
     </row>
@@ -3025,10 +3066,10 @@
         <v>19</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E63" s="23"/>
     </row>
@@ -3041,10 +3082,10 @@
         <v>20</v>
       </c>
       <c r="C64" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D64" s="43" t="s">
         <v>199</v>
-      </c>
-      <c r="D64" s="43" t="s">
-        <v>200</v>
       </c>
       <c r="E64" s="35"/>
       <c r="F64" s="16"/>
@@ -3068,13 +3109,13 @@
         <v>CQ64</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C65" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="42" t="s">
         <v>204</v>
-      </c>
-      <c r="D65" s="42" t="s">
-        <v>205</v>
       </c>
       <c r="E65" s="11"/>
     </row>
@@ -3084,13 +3125,13 @@
         <v>CQ65</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E66" s="11"/>
     </row>
@@ -3100,13 +3141,13 @@
         <v>CQ66</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D67" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E67" s="11"/>
     </row>
@@ -3116,13 +3157,13 @@
         <v>CQ67</v>
       </c>
       <c r="B68" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" s="46" t="s">
         <v>210</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D68" s="46" t="s">
-        <v>211</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>22</v>
@@ -3134,13 +3175,13 @@
         <v>CQ68</v>
       </c>
       <c r="B69" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="D69" s="38" t="s">
         <v>219</v>
-      </c>
-      <c r="D69" s="38" t="s">
-        <v>220</v>
       </c>
       <c r="E69" s="17"/>
     </row>
@@ -3150,11 +3191,11 @@
         <v>CQ69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E70" s="9"/>
     </row>
@@ -3164,7 +3205,7 @@
         <v>CQ70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -3176,7 +3217,7 @@
         <v>CQ71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -3188,32 +3229,55 @@
         <v>CQ72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
     </row>
-    <row r="74" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
+    <row r="74" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ73</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>234</v>
+      </c>
       <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
-      <c r="B75" s="15"/>
+      <c r="E74" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ74</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-    </row>
-    <row r="76" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="14"/>
-      <c r="B76" s="15"/>
+      <c r="E75" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ75</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>233</v>
+      </c>
       <c r="C76" s="15"/>
       <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
+      <c r="E76" s="15" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="77" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="14"/>
@@ -4099,5 +4163,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix #11, Fix #10, Fix #8, Fix #3, Fix #6
Fixed description with the right domain and range, added funcional properties, updated requirements.
</commit_message>
<xml_diff>
--- a/requirements/requirements.xlsx
+++ b/requirements/requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="253">
   <si>
     <t>CQ ID</t>
   </si>
@@ -748,6 +748,36 @@
   </si>
   <si>
     <t>sd:position</t>
+  </si>
+  <si>
+    <t>What are the usage notes of a software component?</t>
+  </si>
+  <si>
+    <t>What is the funding project number?</t>
+  </si>
+  <si>
+    <t>Are there any setups for a software?</t>
+  </si>
+  <si>
+    <t>Is there any example of this software?</t>
+  </si>
+  <si>
+    <t>What are the parameters that are adjustable in a configuration?</t>
+  </si>
+  <si>
+    <t>sd:adjustableParameter</t>
+  </si>
+  <si>
+    <t>sd:example</t>
+  </si>
+  <si>
+    <t>sd:hasSetup</t>
+  </si>
+  <si>
+    <t>sd:fundingGrant</t>
+  </si>
+  <si>
+    <t>sd:hasUsageNotes</t>
   </si>
 </sst>
 </file>
@@ -765,11 +795,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1465,7 +1497,7 @@
   <dimension ref="A1:S202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2511,7 +2543,7 @@
     </row>
     <row r="36" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="str">
-        <f t="shared" ref="A36:A79" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
+        <f t="shared" ref="A36:A83" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
         <v>CQ35</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -3339,39 +3371,71 @@
       </c>
       <c r="E79" s="15"/>
     </row>
-    <row r="80" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="14"/>
-      <c r="B80" s="19"/>
+    <row r="80" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ79</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>243</v>
+      </c>
       <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
+      <c r="D80" s="12" t="s">
+        <v>252</v>
+      </c>
       <c r="E80" s="15"/>
     </row>
-    <row r="81" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="14"/>
-      <c r="B81" s="19"/>
+    <row r="81" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A81" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ80</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>244</v>
+      </c>
       <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
+      <c r="D81" s="12" t="s">
+        <v>251</v>
+      </c>
       <c r="E81" s="15"/>
     </row>
-    <row r="82" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="14"/>
-      <c r="B82" s="19"/>
+    <row r="82" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ81</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>245</v>
+      </c>
       <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
+      <c r="D82" s="12" t="s">
+        <v>250</v>
+      </c>
       <c r="E82" s="15"/>
     </row>
-    <row r="83" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="14"/>
-      <c r="B83" s="19"/>
+    <row r="83" spans="1:5" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A83" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ82</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>246</v>
+      </c>
       <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
+      <c r="D83" s="12" t="s">
+        <v>249</v>
+      </c>
       <c r="E83" s="15"/>
     </row>
     <row r="84" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="14"/>
-      <c r="B84" s="19"/>
+      <c r="B84" s="19" t="s">
+        <v>247</v>
+      </c>
       <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
+      <c r="D84" s="15" t="s">
+        <v>248</v>
+      </c>
       <c r="E84" s="15"/>
     </row>
     <row r="85" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
drafting changes for 1.7.0
</commit_message>
<xml_diff>
--- a/requirements/requirements.xlsx
+++ b/requirements/requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="288">
   <si>
     <t>CQ ID</t>
   </si>
@@ -825,9 +825,6 @@
     <t>Adds a value to increment a parameter: e.g., increment rain by 10% one ach execution</t>
   </si>
   <si>
-    <t>CQ90</t>
-  </si>
-  <si>
     <t>What are the data transformations associated with an input</t>
   </si>
   <si>
@@ -835,6 +832,57 @@
   </si>
   <si>
     <t>Added two different classes extending SoftwareConfiguration and SoftwareConfigurationSetup</t>
+  </si>
+  <si>
+    <t>Where should I have this input placed in order to execute this program?</t>
+  </si>
+  <si>
+    <t>What are the execution instructions of a software component?</t>
+  </si>
+  <si>
+    <t>What are the download instructions for a software component?</t>
+  </si>
+  <si>
+    <t>Where is the readme for this software?</t>
+  </si>
+  <si>
+    <t>Is there an issue tracker that I can use to see open issues?</t>
+  </si>
+  <si>
+    <t>sd:pathLocation</t>
+  </si>
+  <si>
+    <t>sd:executionInstructions</t>
+  </si>
+  <si>
+    <t>sd:downloadInstructions</t>
+  </si>
+  <si>
+    <t>sd:readme</t>
+  </si>
+  <si>
+    <t>sd:issueTracker</t>
+  </si>
+  <si>
+    <t>When extracting metadata from readmes, it is often to see how to execute a software component from a human-readable point of view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructions needed to download a software component </t>
+  </si>
+  <si>
+    <t>Needed to track the source of most documentation (but not all documentation)</t>
+  </si>
+  <si>
+    <t>Is there a Dockerfile for this Software image?</t>
+  </si>
+  <si>
+    <t>Can I find notebooks that illustrate how to use this software?</t>
+  </si>
+  <si>
+    <t>sd:hasExecutableNotebook</t>
+  </si>
+  <si>
+    <t>sd:hasBuildFile</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1186,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1269,6 +1317,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1553,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2600,7 +2649,7 @@
     </row>
     <row r="36" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="str">
-        <f t="shared" ref="A36:A90" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
+        <f t="shared" ref="A36:A98" si="1">CONCATENATE("CQ",ROW(A36)-1)</f>
         <v>CQ35</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -3589,67 +3638,123 @@
       <c r="E90" s="15"/>
     </row>
     <row r="91" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="20" t="s">
+      <c r="A91" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ90</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>268</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>269</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E91" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="E91" s="15" t="s">
+    </row>
+    <row r="92" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ91</v>
+      </c>
+      <c r="B92" s="19" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="14"/>
-      <c r="B92" s="19"/>
       <c r="C92" s="15"/>
-      <c r="D92" s="15"/>
+      <c r="D92" s="12" t="s">
+        <v>276</v>
+      </c>
       <c r="E92" s="15"/>
     </row>
     <row r="93" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="14"/>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
+      <c r="A93" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ92</v>
+      </c>
+      <c r="B93" s="50" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="E93" s="15"/>
     </row>
     <row r="94" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="14"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="15"/>
+      <c r="A94" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ93</v>
+      </c>
+      <c r="B94" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>278</v>
+      </c>
       <c r="E94" s="15"/>
     </row>
     <row r="95" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="14"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="15"/>
+      <c r="A95" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ94</v>
+      </c>
+      <c r="B95" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>279</v>
+      </c>
       <c r="E95" s="15"/>
     </row>
     <row r="96" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="14"/>
-      <c r="B96" s="12"/>
+      <c r="A96" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ95</v>
+      </c>
+      <c r="B96" s="50" t="s">
+        <v>275</v>
+      </c>
       <c r="C96" s="12"/>
-      <c r="D96" s="15"/>
+      <c r="D96" s="12" t="s">
+        <v>280</v>
+      </c>
       <c r="E96" s="15"/>
     </row>
     <row r="97" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="14"/>
-      <c r="B97" s="12"/>
+      <c r="A97" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ96</v>
+      </c>
+      <c r="B97" s="50" t="s">
+        <v>284</v>
+      </c>
       <c r="C97" s="9"/>
-      <c r="D97" s="15"/>
+      <c r="D97" s="12" t="s">
+        <v>287</v>
+      </c>
       <c r="E97" s="15"/>
     </row>
     <row r="98" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="14"/>
-      <c r="B98" s="12"/>
+      <c r="A98" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>CQ97</v>
+      </c>
+      <c r="B98" s="50" t="s">
+        <v>285</v>
+      </c>
       <c r="C98" s="12"/>
-      <c r="D98" s="15"/>
+      <c r="D98" s="12" t="s">
+        <v>286</v>
+      </c>
       <c r="E98" s="15"/>
     </row>
     <row r="99" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>